<commit_message>
play with distance and metric
</commit_message>
<xml_diff>
--- a/f1score_merlin_abnormal_point_results.xlsx
+++ b/f1score_merlin_abnormal_point_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,120 +436,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.19</t>
+          <t>our_identified</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.18</t>
+          <t>our_Overlap_merlin</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.17</t>
+          <t>ourbest_param</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.16</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.15</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.14</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.13</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.12</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.11</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.10</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.9</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.8</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.7</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.6</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.5</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.4</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.3</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.2</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0.1</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 0</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>our_identified</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>our_Overlap_merlin</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>ourbest_param</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>ourtime_taken</t>
         </is>
@@ -559,81 +459,21 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>{'cluster': 26, 'training': 386, 'window': 362, 'threshold': 1.5}</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>{'cluster': 19, 'training': 1456, 'window': 362, 'threshold': 9.5}</t>
-        </is>
-      </c>
-      <c r="Y2" t="n">
-        <v>21.95178538099935</v>
+        <v>20.03201633800199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test on UCR anomaly dataset but got score 0
</commit_message>
<xml_diff>
--- a/f1score_merlin_abnormal_point_results.xlsx
+++ b/f1score_merlin_abnormal_point_results.xlsx
@@ -469,11 +469,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'cluster': 29, 'training': 83, 'window': 362, 'threshold': 3.5}</t>
+          <t>{'cluster': 12, 'training': 571, 'window': 102, 'threshold': 5.5}</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>22.48344128600002</v>
+        <v>341.2996447039986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>